<commit_message>
edit xlsx and xlsx2Json.js
</commit_message>
<xml_diff>
--- a/xlsx/sample.xlsx
+++ b/xlsx/sample.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="product" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="seller" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="product_master" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="seller_master" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="product" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -62,6 +63,18 @@
     <t xml:space="preserve">product5</t>
   </si>
   <si>
+    <t xml:space="preserve">00006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product7</t>
+  </si>
+  <si>
     <t xml:space="preserve">tel</t>
   </si>
   <si>
@@ -108,6 +121,12 @@
   </si>
   <si>
     <t xml:space="preserve">03-567-8901</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seller_id</t>
   </si>
 </sst>
 </file>
@@ -123,6 +142,7 @@
       <sz val="10"/>
       <name val="Hiragino Mincho ProN"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -144,47 +164,55 @@
       <color rgb="FF000000"/>
       <name val="Hiragino Mincho ProN"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Hiragino Mincho ProN"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF808080"/>
       <name val="Hiragino Mincho ProN"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF006600"/>
       <name val="Hiragino Mincho ProN"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
       <name val="Hiragino Mincho ProN"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFCC0000"/>
       <name val="Hiragino Mincho ProN"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Hiragino Mincho ProN"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -291,24 +319,56 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -322,6 +382,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -426,19 +490,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="69" zoomScaleNormal="69" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.87"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -448,61 +512,91 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>500</v>
       </c>
+      <c r="D2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>600</v>
       </c>
+      <c r="D3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>700</v>
       </c>
+      <c r="D4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>800</v>
       </c>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>900</v>
       </c>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>1100</v>
+      </c>
+      <c r="D8" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -522,17 +616,17 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="69" zoomScaleNormal="69" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="69" zoomScaleNormal="69" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="10.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="10.87"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -540,68 +634,165 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>16</v>
+      <c r="A2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>19</v>
+      <c r="A3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>22</v>
+      <c r="A4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>25</v>
+      <c r="A5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>28</v>
+      <c r="A6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="69" zoomScaleNormal="69" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="10.87"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>